<commit_message>
Demo Versie voor Valencia
</commit_message>
<xml_diff>
--- a/project-root/data/location-data.xlsx
+++ b/project-root/data/location-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maart\EigenMappen\greenTravelMap\greentu-travelmap\project-root\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECC3C8C-FA8C-4CBB-AE02-3C23CA5AD3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53B8C99-EC63-4607-9E9D-2D016933D0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{ECCE8C5B-07D3-478B-A9F2-74E552C64914}"/>
   </bookViews>
@@ -1109,9 +1109,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7254D566-3C65-4661-BAE0-38210166E19C}">
   <dimension ref="A1:BS1167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="79" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L1" sqref="L1"/>
+      <selection pane="topRight" activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2062,7 +2062,7 @@
         <v>-0.37628810000000001</v>
       </c>
       <c r="O27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -2272,7 +2272,7 @@
         <v>4.3516969999999997</v>
       </c>
       <c r="O35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
@@ -3099,7 +3099,7 @@
         <v>16.372504200000002</v>
       </c>
       <c r="O63" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>